<commit_message>
correct nominal values, variation coefficients and resulting input concentrations
</commit_message>
<xml_diff>
--- a/documentation/bmp_analysis_Hafner_2018.xlsx
+++ b/documentation/bmp_analysis_Hafner_2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\SimonsHardDriveSpeicher\GIT\ad_meal_prep_control\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68C565D-BEF5-4FF9-AF55-DA962E24777F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577FB0E7-0ED7-4443-8559-85866696DDDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{A9FF6FE0-0DD8-4EC1-B47A-C69099783B76}"/>
   </bookViews>
@@ -80,7 +80,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>